<commit_message>
Add report generator and HTML outputs
</commit_message>
<xml_diff>
--- a/cline-costs.xlsx
+++ b/cline-costs.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="API Calls" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Summary" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Summary1" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Summary2" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Summary3" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Summary4" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Summary5" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="Summary6" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="Summary7" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="API Calls" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary1" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary2" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary3" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary4" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary5" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary6" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary7" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary8" sheetId="10" state="visible" r:id="rId10"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -444,7 +445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -976,6 +977,221 @@
       </c>
       <c r="I13" t="n">
         <v>10.580807</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2025-12-15 14:19:40</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Remote/SSH Cline</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Smoothie_Bar_IG</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>right now i have a generate_report script that takes a standard word doc and makes it into an HTML f</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>claude-sonnet-3-5</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
+        <v>1506903</v>
+      </c>
+      <c r="G14" t="n">
+        <v>62835</v>
+      </c>
+      <c r="H14" t="n">
+        <v>13.435237</v>
+      </c>
+      <c r="I14" t="n">
+        <v>24.016044</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2025-12-15 19:34:46</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Remote/SSH Cline</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Smoothie_Bar_IG</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">i am making a script that transforms this word doc as a template to html for presentation.   i want </t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>claude-sonnet-3-5</t>
+        </is>
+      </c>
+      <c r="F15" t="n">
+        <v>1917669</v>
+      </c>
+      <c r="G15" t="n">
+        <v>46976</v>
+      </c>
+      <c r="H15" t="n">
+        <v>16.337973</v>
+      </c>
+      <c r="I15" t="n">
+        <v>40.354017</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="30" customWidth="1" min="1" max="1"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>Metric</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Total API Calls</t>
+        </is>
+      </c>
+      <c r="B2" s="3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>- Cline Coding Calls</t>
+        </is>
+      </c>
+      <c r="B3" s="3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>- Automated Analysis Calls</t>
+        </is>
+      </c>
+      <c r="B4" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Average Cost per Call (All)</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t>$20.177009</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>- Avg Coding Call Cost</t>
+        </is>
+      </c>
+      <c r="B6" s="3" t="inlineStr">
+        <is>
+          <t>$14.886605</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>- Avg Analysis Call Cost</t>
+        </is>
+      </c>
+      <c r="B7" s="3" t="inlineStr">
+        <is>
+          <t>$0.000000</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Total Cost</t>
+        </is>
+      </c>
+      <c r="B8" s="3" t="inlineStr">
+        <is>
+          <t>$40.354017</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>- Coding Cost</t>
+        </is>
+      </c>
+      <c r="B9" s="3" t="inlineStr">
+        <is>
+          <t>$29.773210</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>- Analysis Cost</t>
+        </is>
+      </c>
+      <c r="B10" s="3" t="inlineStr">
+        <is>
+          <t>$0.000000</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>